<commit_message>
update upload student file
</commit_message>
<xml_diff>
--- a/Edu-Mgmt-BE/Files/import-student.xlsx
+++ b/Edu-Mgmt-BE/Files/import-student.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workplace\C#\Edu-Mgmt-BE\Edu-Mgmt-BE\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24B39F1C-395C-445A-99F8-A5111EA0BA36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F714FB-4B5A-45C0-B491-E0F8D8EA5E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="1425" windowWidth="21600" windowHeight="11385" xr2:uid="{0733CDB4-CC3A-456E-BCE4-4CA191C8B14F}"/>
+    <workbookView xWindow="-23460" yWindow="1410" windowWidth="21600" windowHeight="11385" xr2:uid="{0733CDB4-CC3A-456E-BCE4-4CA191C8B14F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -570,7 +570,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
replace student excel format file
</commit_message>
<xml_diff>
--- a/Edu-Mgmt-BE/Files/import-student.xlsx
+++ b/Edu-Mgmt-BE/Files/import-student.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workplace\C#\Edu-Mgmt-BE\Edu-Mgmt-BE\Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hoag\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7F714FB-4B5A-45C0-B491-E0F8D8EA5E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3CFBAC1-3528-4BDD-A628-AF5DC982B4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23460" yWindow="1410" windowWidth="21600" windowHeight="11385" xr2:uid="{0733CDB4-CC3A-456E-BCE4-4CA191C8B14F}"/>
+    <workbookView xWindow="5820" yWindow="2175" windowWidth="21600" windowHeight="11385" xr2:uid="{0733CDB4-CC3A-456E-BCE4-4CA191C8B14F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,10 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="51">
-  <si>
-    <t xml:space="preserve">21CL73402010001 </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>Khuất Thùy An</t>
   </si>
@@ -47,15 +44,9 @@
     <t xml:space="preserve">0357697280                                                      </t>
   </si>
   <si>
-    <t>Thuế - Hải quan</t>
-  </si>
-  <si>
     <t>Hà Nội</t>
   </si>
   <si>
-    <t xml:space="preserve">21CL73402010002 </t>
-  </si>
-  <si>
     <t>Nguyễn Nguyên Anh</t>
   </si>
   <si>
@@ -65,99 +56,66 @@
     <t xml:space="preserve">0832882003                                                      </t>
   </si>
   <si>
-    <t xml:space="preserve">21CL73402010003 </t>
-  </si>
-  <si>
     <t>Nguyễn Việt Anh</t>
   </si>
   <si>
     <t xml:space="preserve">086 5352526                                                     </t>
   </si>
   <si>
-    <t xml:space="preserve">21CL73402010004 </t>
-  </si>
-  <si>
     <t>Trương Nguyễn Đức Anh</t>
   </si>
   <si>
     <t xml:space="preserve">0827101510                                                      </t>
   </si>
   <si>
-    <t xml:space="preserve">21CL73402010005 </t>
-  </si>
-  <si>
     <t>Đặng Hải Châu</t>
   </si>
   <si>
     <t xml:space="preserve">0961303703                                                      </t>
   </si>
   <si>
-    <t xml:space="preserve">21CL73402010647 </t>
-  </si>
-  <si>
     <t>Nguyễn Minh Châu</t>
   </si>
   <si>
     <t xml:space="preserve">0389219388                                                      </t>
   </si>
   <si>
-    <t xml:space="preserve">21CL73402010006 </t>
-  </si>
-  <si>
     <t>Nguyễn Thị Dinh Dinh</t>
   </si>
   <si>
     <t xml:space="preserve">0704809463                                                      </t>
   </si>
   <si>
-    <t xml:space="preserve">21CL73402010007 </t>
-  </si>
-  <si>
     <t>Nguyễn Phan Thùy Dương</t>
   </si>
   <si>
     <t xml:space="preserve">0972233081                                                      </t>
   </si>
   <si>
-    <t xml:space="preserve">21CL73402010008 </t>
-  </si>
-  <si>
     <t>Phạm Ngọc Hà</t>
   </si>
   <si>
     <t>0912017315</t>
   </si>
   <si>
-    <t xml:space="preserve">21CL73402010009 </t>
-  </si>
-  <si>
     <t>Đoàn Hồng Hải</t>
   </si>
   <si>
     <t xml:space="preserve">0981569559                                                      </t>
   </si>
   <si>
-    <t xml:space="preserve">21CL73402010010 </t>
-  </si>
-  <si>
     <t>Trần Vũ Thu Hằng</t>
   </si>
   <si>
     <t xml:space="preserve">0987538034                                                      </t>
   </si>
   <si>
-    <t xml:space="preserve">21CL73402010011 </t>
-  </si>
-  <si>
     <t>Vũ Đức Hiếu</t>
   </si>
   <si>
     <t xml:space="preserve">0355677469                                                      </t>
   </si>
   <si>
-    <t xml:space="preserve">21CL73402010012 </t>
-  </si>
-  <si>
     <t>Đặng Việt Hưng</t>
   </si>
   <si>
@@ -167,9 +125,6 @@
     <t>STT</t>
   </si>
   <si>
-    <t>Mã học sinh</t>
-  </si>
-  <si>
     <t>Họ tên</t>
   </si>
   <si>
@@ -180,9 +135,6 @@
   </si>
   <si>
     <t>Số điện thoại</t>
-  </si>
-  <si>
-    <t>Mô tả</t>
   </si>
   <si>
     <t>Địa chỉ</t>
@@ -567,382 +519,298 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDEF87CC-89F5-47B9-BCB3-393594930297}">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="4">
+        <v>37942</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4">
-        <v>37942</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="4">
+        <v>37861</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="F3" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="C4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>37864</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="4">
-        <v>37861</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="4">
-        <v>37864</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F4" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4">
         <v>37909</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
         <v>37805</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4">
         <v>37979</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
         <v>37630</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E9" s="4">
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="4">
         <v>37785</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4">
         <v>37753</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4">
         <v>37956</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4">
         <v>37881</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E13" s="4">
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4">
         <v>37659</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E13" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="4">
+      <c r="B14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="4">
         <v>37755</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>5</v>
+      <c r="E14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>